<commit_message>
analysis completed - conclusions remain
</commit_message>
<xml_diff>
--- a/apgar5unhealthy.xlsx
+++ b/apgar5unhealthy.xlsx
@@ -482,25 +482,17 @@
       <c r="C2" t="n">
         <v>7.14</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=12.694569646310693)</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=12.694569646310693)</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=12.694569646310693)</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=12.694569646310693)</t>
-        </is>
+      <c r="D2" t="n">
+        <v>13.10423286807256</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.025939589265073</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3.37347590611476</v>
+      </c>
+      <c r="G2" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="3">
@@ -515,25 +507,17 @@
       <c r="C3" t="n">
         <v>7.13</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=21.61786778997403)</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=21.61786778997403)</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=21.61786778997403)</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=21.61786778997403)</t>
-        </is>
+      <c r="D3" t="n">
+        <v>22.29447150050382</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.626556528030944</v>
+      </c>
+      <c r="F3" t="n">
+        <v>14.58340096931597</v>
+      </c>
+      <c r="G3" t="n">
+        <v>86</v>
       </c>
     </row>
     <row r="4">
@@ -548,25 +532,17 @@
       <c r="C4" t="n">
         <v>7.12</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=11.123000725748929)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=11.123000725748929)</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=11.123000725748929)</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=11.123000725748929)</t>
-        </is>
+      <c r="D4" t="n">
+        <v>11.43705331809856</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.920757794620315</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4.20277796320079</v>
+      </c>
+      <c r="G4" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="5">
@@ -581,25 +557,17 @@
       <c r="C5" t="n">
         <v>7.03</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=10.648900234541857)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=10.648900234541857)</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=10.648900234541857)</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=10.648900234541857)</t>
-        </is>
+      <c r="D5" t="n">
+        <v>10.64927355675065</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.7650142517193413</v>
+      </c>
+      <c r="F5" t="n">
+        <v>7.006603063537734</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -614,25 +582,17 @@
       <c r="C6" t="n">
         <v>7.26</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=15.608012152621097)</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=15.608012152621097)</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=15.608012152621097)</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=15.608012152621097)</t>
-        </is>
+      <c r="D6" t="n">
+        <v>16.02409046434199</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.174723496625334</v>
+      </c>
+      <c r="F6" t="n">
+        <v>6.040278558458219</v>
+      </c>
+      <c r="G6" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="7">
@@ -647,25 +607,17 @@
       <c r="C7" t="n">
         <v>7.28</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=8.115459341762605)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=8.115459341762605)</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=8.115459341762605)</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=8.115459341762605)</t>
-        </is>
+      <c r="D7" t="n">
+        <v>8.113389967505748</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.396139937127157</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4.685676507111217</v>
+      </c>
+      <c r="G7" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -680,25 +632,17 @@
       <c r="C8" t="n">
         <v>7.18</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=19.098460492485643)</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=19.098460492485643)</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=19.098460492485643)</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=19.098460492485643)</t>
-        </is>
+      <c r="D8" t="n">
+        <v>19.11824566937721</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.6266717308582</v>
+      </c>
+      <c r="F8" t="n">
+        <v>13.57207349789775</v>
+      </c>
+      <c r="G8" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -713,25 +657,17 @@
       <c r="C9" t="n">
         <v>7.07</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=15.712501702371974)</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=15.712501702371974)</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=15.712501702371974)</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=15.712501702371974)</t>
-        </is>
+      <c r="D9" t="n">
+        <v>16.03109597208861</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2.206187332209771</v>
+      </c>
+      <c r="F9" t="n">
+        <v>7.832334238509944</v>
+      </c>
+      <c r="G9" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="10">
@@ -746,25 +682,17 @@
       <c r="C10" t="n">
         <v>7.2</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=18.04051762605019)</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=18.04051762605019)</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=18.04051762605019)</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>ReturnTuple(sdnn=18.04051762605019)</t>
-        </is>
+      <c r="D10" t="n">
+        <v>18.04385261486464</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3.155559826166355</v>
+      </c>
+      <c r="F10" t="n">
+        <v>6.328767076480719</v>
+      </c>
+      <c r="G10" t="n">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>